<commit_message>
Complete Explicit wait and programming language
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -502,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,11 @@
           <t>school</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -558,6 +563,11 @@
           <t>西安电子科技大学</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -586,6 +596,11 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>Chinese National Table Tennis Team</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>C++</t>
         </is>
       </c>
     </row>
@@ -610,6 +625,11 @@
           <t>杭州电子科技大学</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -628,6 +648,11 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -650,6 +675,11 @@
           <t>浙江大学</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -678,6 +708,11 @@
       <c r="F7" t="inlineStr">
         <is>
           <t>University of Science and Technology of China</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Python</t>
         </is>
       </c>
     </row>
@@ -698,6 +733,11 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -720,6 +760,11 @@
           <t>清华大学</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -742,6 +787,11 @@
           <t>汕头大学</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -760,6 +810,11 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -778,6 +833,11 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -804,6 +864,11 @@
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -826,6 +891,11 @@
           <t>南开大学</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -844,6 +914,11 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -862,6 +937,11 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -880,6 +960,11 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>JavaScript</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -898,6 +983,11 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -916,6 +1006,11 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -944,6 +1039,11 @@
       <c r="F20" t="inlineStr">
         <is>
           <t>University of British Columbia</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Java</t>
         </is>
       </c>
     </row>
@@ -968,6 +1068,11 @@
           <t>NIT Silchar</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -996,6 +1101,11 @@
       <c r="F22" t="inlineStr">
         <is>
           <t>浙江大学</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>C++</t>
         </is>
       </c>
     </row>
@@ -1020,6 +1130,11 @@
           <t>清华大学</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Python</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -1042,6 +1157,11 @@
           <t>南京大学</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -1060,6 +1180,11 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>C++</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -1078,6 +1203,11 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Python3</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>